<commit_message>
Update 2020-weekly data & cleanup
</commit_message>
<xml_diff>
--- a/notebooks/out/2020 Primary Weekly Analysis.xlsx
+++ b/notebooks/out/2020 Primary Weekly Analysis.xlsx
@@ -425,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,10 +483,10 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C2">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="D2">
         <v>136</v>
@@ -495,34 +495,34 @@
         <v>18</v>
       </c>
       <c r="F2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G2">
         <v>723</v>
       </c>
       <c r="H2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1104</v>
+        <v>1097</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>1118</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -530,10 +530,10 @@
         <v>43897</v>
       </c>
       <c r="B3">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -545,13 +545,13 @@
         <v>11</v>
       </c>
       <c r="G3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3">
         <v>33</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1223</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -577,25 +577,25 @@
         <v>43904</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>33</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -604,10 +604,10 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>26</v>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="O4">
-        <v>1279</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -624,34 +624,34 @@
         <v>43911</v>
       </c>
       <c r="B5">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C5">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H5">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -660,10 +660,10 @@
         <v>11</v>
       </c>
       <c r="N5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O5">
-        <v>1398</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -671,25 +671,25 @@
         <v>43918</v>
       </c>
       <c r="B6">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C6">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H6">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I6">
         <v>13</v>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -707,10 +707,10 @@
         <v>13</v>
       </c>
       <c r="N6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O6">
-        <v>1673</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -718,34 +718,34 @@
         <v>43925</v>
       </c>
       <c r="B7">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="C7">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="D7">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="H7">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="O7">
-        <v>1997</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -765,34 +765,34 @@
         <v>43932</v>
       </c>
       <c r="B8">
-        <v>1442</v>
+        <v>1570</v>
       </c>
       <c r="C8">
-        <v>1184</v>
+        <v>1281</v>
       </c>
       <c r="D8">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="E8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="G8">
-        <v>1196</v>
+        <v>1258</v>
       </c>
       <c r="H8">
-        <v>246</v>
+        <v>312</v>
       </c>
       <c r="I8">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1305</v>
+        <v>1415</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -801,10 +801,10 @@
         <v>18</v>
       </c>
       <c r="N8">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="O8">
-        <v>3439</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -812,46 +812,46 @@
         <v>43939</v>
       </c>
       <c r="B9">
-        <v>2656</v>
+        <v>2798</v>
       </c>
       <c r="C9">
-        <v>2137</v>
+        <v>2247</v>
       </c>
       <c r="D9">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="E9">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="G9">
-        <v>2190</v>
+        <v>2251</v>
       </c>
       <c r="H9">
-        <v>466</v>
+        <v>547</v>
       </c>
       <c r="I9">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>2221</v>
+        <v>2351</v>
       </c>
       <c r="L9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>17</v>
       </c>
       <c r="N9">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="O9">
-        <v>6095</v>
+        <v>6405</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -859,34 +859,34 @@
         <v>43946</v>
       </c>
       <c r="B10">
-        <v>2479</v>
+        <v>2574</v>
       </c>
       <c r="C10">
-        <v>1884</v>
+        <v>1969</v>
       </c>
       <c r="D10">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="E10">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G10">
-        <v>1885</v>
+        <v>1891</v>
       </c>
       <c r="H10">
-        <v>594</v>
+        <v>683</v>
       </c>
       <c r="I10">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>2025</v>
+        <v>2107</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -895,10 +895,10 @@
         <v>11</v>
       </c>
       <c r="N10">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="O10">
-        <v>8574</v>
+        <v>8979</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -906,34 +906,34 @@
         <v>43953</v>
       </c>
       <c r="B11">
-        <v>2603</v>
+        <v>2748</v>
       </c>
       <c r="C11">
-        <v>1952</v>
+        <v>2052</v>
       </c>
       <c r="D11">
-        <v>305</v>
+        <v>327</v>
       </c>
       <c r="E11">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F11">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="G11">
-        <v>2054</v>
+        <v>2115</v>
       </c>
       <c r="H11">
-        <v>549</v>
+        <v>633</v>
       </c>
       <c r="I11">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>2016</v>
+        <v>2141</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -942,10 +942,10 @@
         <v>21</v>
       </c>
       <c r="N11">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="O11">
-        <v>11177</v>
+        <v>11727</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -953,34 +953,34 @@
         <v>43960</v>
       </c>
       <c r="B12">
-        <v>4169</v>
+        <v>4435</v>
       </c>
       <c r="C12">
-        <v>3309</v>
+        <v>3524</v>
       </c>
       <c r="D12">
-        <v>374</v>
+        <v>404</v>
       </c>
       <c r="E12">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12">
-        <v>432</v>
+        <v>452</v>
       </c>
       <c r="G12">
-        <v>3493</v>
+        <v>3586</v>
       </c>
       <c r="H12">
-        <v>676</v>
+        <v>849</v>
       </c>
       <c r="I12">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>3446</v>
+        <v>3680</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -989,10 +989,10 @@
         <v>26</v>
       </c>
       <c r="N12">
-        <v>402</v>
+        <v>430</v>
       </c>
       <c r="O12">
-        <v>15346</v>
+        <v>16162</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1000,46 +1000,46 @@
         <v>43967</v>
       </c>
       <c r="B13">
-        <v>4742</v>
+        <v>4988</v>
       </c>
       <c r="C13">
-        <v>3644</v>
+        <v>3836</v>
       </c>
       <c r="D13">
-        <v>522</v>
+        <v>552</v>
       </c>
       <c r="E13">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F13">
-        <v>498</v>
+        <v>520</v>
       </c>
       <c r="G13">
-        <v>3637</v>
+        <v>3710</v>
       </c>
       <c r="H13">
-        <v>1105</v>
+        <v>1278</v>
       </c>
       <c r="I13">
-        <v>484</v>
+        <v>505</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>3683</v>
+        <v>3883</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>41</v>
       </c>
       <c r="N13">
-        <v>533</v>
+        <v>559</v>
       </c>
       <c r="O13">
-        <v>20088</v>
+        <v>21150</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1047,34 +1047,34 @@
         <v>43974</v>
       </c>
       <c r="B14">
-        <v>5662</v>
+        <v>6056</v>
       </c>
       <c r="C14">
-        <v>4294</v>
+        <v>4582</v>
       </c>
       <c r="D14">
-        <v>655</v>
+        <v>730</v>
       </c>
       <c r="E14">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F14">
-        <v>615</v>
+        <v>644</v>
       </c>
       <c r="G14">
-        <v>4144</v>
+        <v>4285</v>
       </c>
       <c r="H14">
-        <v>1518</v>
+        <v>1771</v>
       </c>
       <c r="I14">
-        <v>520</v>
+        <v>555</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>4355</v>
+        <v>4659</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1083,10 +1083,10 @@
         <v>30</v>
       </c>
       <c r="N14">
-        <v>756</v>
+        <v>811</v>
       </c>
       <c r="O14">
-        <v>25750</v>
+        <v>27206</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1094,46 +1094,46 @@
         <v>43981</v>
       </c>
       <c r="B15">
-        <v>8294</v>
+        <v>9133</v>
       </c>
       <c r="C15">
-        <v>6306</v>
+        <v>6961</v>
       </c>
       <c r="D15">
-        <v>1023</v>
+        <v>1129</v>
       </c>
       <c r="E15">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F15">
-        <v>834</v>
+        <v>901</v>
       </c>
       <c r="G15">
-        <v>5967</v>
+        <v>6276</v>
       </c>
       <c r="H15">
-        <v>2327</v>
+        <v>2857</v>
       </c>
       <c r="I15">
-        <v>753</v>
+        <v>846</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>6182</v>
+        <v>6767</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>1357</v>
+        <v>1519</v>
       </c>
       <c r="O15">
-        <v>34044</v>
+        <v>36339</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1141,92 +1141,233 @@
         <v>43988</v>
       </c>
       <c r="B16">
-        <v>4550</v>
+        <v>18703</v>
       </c>
       <c r="C16">
-        <v>3763</v>
+        <v>14597</v>
       </c>
       <c r="D16">
-        <v>363</v>
+        <v>2047</v>
       </c>
       <c r="E16">
-        <v>58</v>
+        <v>257</v>
       </c>
       <c r="F16">
-        <v>366</v>
+        <v>1802</v>
       </c>
       <c r="G16">
-        <v>3447</v>
+        <v>13588</v>
       </c>
       <c r="H16">
-        <v>1103</v>
+        <v>5115</v>
       </c>
       <c r="I16">
-        <v>484</v>
+        <v>2128</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>3050</v>
+        <v>13456</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="N16">
-        <v>1015</v>
+        <v>3093</v>
       </c>
       <c r="O16">
-        <v>38594</v>
+        <v>55042</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
+      <c r="A17" s="2">
+        <v>43995</v>
       </c>
       <c r="B17">
-        <v>38594</v>
+        <v>24339</v>
       </c>
       <c r="C17">
-        <v>29949</v>
+        <v>16096</v>
       </c>
       <c r="D17">
-        <v>4077</v>
+        <v>4978</v>
       </c>
       <c r="E17">
-        <v>617</v>
+        <v>415</v>
       </c>
       <c r="F17">
-        <v>3951</v>
+        <v>2850</v>
       </c>
       <c r="G17">
-        <v>29386</v>
+        <v>15376</v>
       </c>
       <c r="H17">
-        <v>9208</v>
+        <v>8963</v>
       </c>
       <c r="I17">
-        <v>3412</v>
+        <v>5466</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>28942</v>
+        <v>14393</v>
       </c>
       <c r="L17">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="M17">
-        <v>1433</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>4798</v>
+        <v>4456</v>
       </c>
       <c r="O17">
+        <v>79381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B18">
+        <v>28771</v>
+      </c>
+      <c r="C18">
+        <v>18876</v>
+      </c>
+      <c r="D18">
+        <v>5407</v>
+      </c>
+      <c r="E18">
+        <v>542</v>
+      </c>
+      <c r="F18">
+        <v>3946</v>
+      </c>
+      <c r="G18">
+        <v>18427</v>
+      </c>
+      <c r="H18">
+        <v>10344</v>
+      </c>
+      <c r="I18">
+        <v>7149</v>
+      </c>
+      <c r="J18">
+        <v>18</v>
+      </c>
+      <c r="K18">
+        <v>15186</v>
+      </c>
+      <c r="L18">
+        <v>571</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>5847</v>
+      </c>
+      <c r="O18">
+        <v>108152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B19">
+        <v>29273</v>
+      </c>
+      <c r="C19">
+        <v>18574</v>
+      </c>
+      <c r="D19">
+        <v>5786</v>
+      </c>
+      <c r="E19">
+        <v>580</v>
+      </c>
+      <c r="F19">
+        <v>4333</v>
+      </c>
+      <c r="G19">
+        <v>18526</v>
+      </c>
+      <c r="H19">
+        <v>10747</v>
+      </c>
+      <c r="I19">
+        <v>9215</v>
+      </c>
+      <c r="J19">
+        <v>77</v>
+      </c>
+      <c r="K19">
+        <v>12498</v>
+      </c>
+      <c r="L19">
+        <v>1318</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>6165</v>
+      </c>
+      <c r="O19">
+        <v>137425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>137425</v>
+      </c>
+      <c r="C20">
+        <v>96098</v>
+      </c>
+      <c r="D20">
+        <v>22244</v>
+      </c>
+      <c r="E20">
+        <v>2380</v>
+      </c>
+      <c r="F20">
+        <v>16703</v>
+      </c>
+      <c r="G20">
+        <v>92678</v>
+      </c>
+      <c r="H20">
+        <v>44747</v>
+      </c>
+      <c r="I20">
+        <v>27068</v>
+      </c>
+      <c r="J20">
+        <v>96</v>
+      </c>
+      <c r="K20">
+        <v>83233</v>
+      </c>
+      <c r="L20">
+        <v>1916</v>
+      </c>
+      <c r="M20">
+        <v>1450</v>
+      </c>
+      <c r="N20">
+        <v>23662</v>
+      </c>
+      <c r="O20">
         <v>0</v>
       </c>
     </row>

</xml_diff>